<commit_message>
Buffer Logic issues rectified
</commit_message>
<xml_diff>
--- a/input_data/input.xlsx
+++ b/input_data/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3rd sem\Eco_ideathon_project\k\Helio_Yajna_Solar_Detection_2\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FD8A2C-9013-4045-BB7B-8E6E5D211B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698971E0-A1CE-4282-B0F8-FECD944DF8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,8 +70,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -377,8 +376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="G127" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G36" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -406,7 +405,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
@@ -417,7 +416,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
@@ -428,7 +427,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
@@ -439,7 +438,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
@@ -450,7 +449,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
@@ -461,7 +460,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
@@ -472,7 +471,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
@@ -483,18 +482,18 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>14.138729</v>
+        <v>21.21746072645459</v>
       </c>
       <c r="C10">
-        <v>77.314622</v>
+        <v>72.894130753303557</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
@@ -505,1333 +504,1333 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>17.254484000000001</v>
+        <v>23.074306857733681</v>
       </c>
       <c r="C12">
-        <v>78.305047000000002</v>
+        <v>72.548291896820118</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>21.110114069556602</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>72.864345885913835</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>21.503045704553202</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>70.459468289688061</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>21.191175925278539</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>72.792899649143209</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>21.136159240459978</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>72.799905715274818</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>21.216949860937302</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>72.903088569450333</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>23.452999743435988</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>71.995765538692496</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>21.24767333600122</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>72.842324083328279</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
         <v>22.98773751244217</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>72.621284608459518</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
         <v>23.00252694624837</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>72.605326120376546</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>23.053969272025959</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>72.559826909786906</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
         <v>22.29917478646448</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>70.759587622020732</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24">
         <v>21.217002585854999</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>72.894881771827684</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
         <v>21.726265898495821</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>70.440289678573592</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26">
         <v>21.218911757346518</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>72.881348926250496</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
         <v>23.066222370555529</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>72.513513467597917</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
         <v>22.03418797591663</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>71.204938716602314</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29">
         <v>21.118628219546618</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>72.842917258930186</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30">
         <v>21.742896949674549</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>70.27153947486876</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31">
         <v>21.760937316510429</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
         <v>70.619127580356604</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32">
         <v>21.237174987330899</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32">
         <v>72.899360050262459</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
         <v>22.980925850442329</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
         <v>72.60870174834065</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34">
         <v>21.168043909697339</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
         <v>72.839121050262463</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35">
         <v>23.06719377261334</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
         <v>72.513180873680099</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36">
         <v>22.975287310786818</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36">
         <v>72.498565946102119</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37">
         <v>21.239913259061769</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37">
         <v>72.908014576721172</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38">
         <v>21.237770662304769</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38">
         <v>72.876444081020338</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="1">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39">
         <v>23.00860571397525</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39">
         <v>72.554649038028714</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="1">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40">
         <v>21.110034724992779</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40">
         <v>72.860541406082163</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="1">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41">
         <v>21.232963604189781</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41">
         <v>72.821899298286397</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="1">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42">
         <v>21.21059453245082</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42">
         <v>72.783302274799368</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="1">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43">
         <v>21.26229880248162</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43">
         <v>72.957983499336251</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="1">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44">
         <v>21.240346160364521</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44">
         <v>72.907612245368966</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="1">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45">
         <v>21.217178826705439</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45">
         <v>72.891703660049473</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46">
         <v>21.22016811429782</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46">
         <v>72.854405364418028</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="1">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47">
         <v>21.215496598424949</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47">
         <v>72.828696559524531</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48">
         <v>23.03919126787812</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48">
         <v>72.661538660049473</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="1">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49">
         <v>23.07479506799794</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49">
         <v>72.56304174966813</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="1">
+      <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50">
         <v>22.95879277823601</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50">
         <v>72.620637958335863</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="1">
+      <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51">
         <v>21.724534099285151</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51">
         <v>70.443933759593932</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="1">
+      <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52">
         <v>22.294925236865421</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52">
         <v>70.756485830688476</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="1">
+      <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53">
         <v>23.107003466221109</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53">
         <v>72.602927923942559</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="1">
+      <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54">
         <v>21.21064739724968</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54">
         <v>72.784147170639017</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="1">
+      <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55">
         <v>21.241180718860509</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55">
         <v>72.876250147151978</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="1">
+      <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56">
         <v>21.218329730283148</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56">
         <v>72.879952478504194</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="1">
+      <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57">
         <v>22.981679072665791</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57">
         <v>72.593846299266858</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="1">
+      <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58">
         <v>21.201502232697141</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58">
         <v>72.874588863754283</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="1">
+      <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59">
         <v>21.215247051468399</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59">
         <v>72.776550942466699</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="1">
+      <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60">
         <v>21.13118638536136</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60">
         <v>72.890363263893093</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" s="1">
+      <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61">
         <v>23.110781017739772</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61">
         <v>72.564691449073791</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="1">
+      <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62">
         <v>23.046389357448231</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62">
         <v>72.660563558197055</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="1">
+      <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63">
         <v>22.377082278034109</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63">
         <v>71.979338660049464</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="1">
+      <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64">
         <v>21.26256303362808</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64">
         <v>72.957975452709206</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="1">
+      <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65">
         <v>21.226124022370559</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65">
         <v>72.929349739742321</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="1">
+      <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66">
         <v>23.008421045875799</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66">
         <v>72.661897374343823</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="1">
+      <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67">
         <v>23.108421833867251</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67">
         <v>72.574231077384923</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="1">
+      <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68">
         <v>23.075783797671669</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68">
         <v>72.563092711639399</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="1">
+      <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69">
         <v>23.06840126925896</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69">
         <v>72.670816149806939</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="1">
+      <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70">
         <v>22.27756751641574</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70">
         <v>70.80376968088153</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="1">
+      <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71">
         <v>22.970480938426562</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C71">
         <v>72.616404549598727</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="1">
+      <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72">
         <v>21.216065694369998</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72">
         <v>72.892563505626654</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="1">
+      <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73">
         <v>21.196885898403441</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73">
         <v>72.780910728836062</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="1">
+      <c r="A74">
         <v>73</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74">
         <v>21.19608529896151</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C74">
         <v>72.78136938657758</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="1">
+      <c r="A75">
         <v>74</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75">
         <v>21.220835200154919</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75">
         <v>72.828906523803752</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="1">
+      <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76">
         <v>22.291899939338869</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76">
         <v>70.79017970800399</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="1">
+      <c r="A77">
         <v>76</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77">
         <v>21.21481510376783</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77">
         <v>72.87400804662704</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="1">
+      <c r="A78">
         <v>77</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78">
         <v>22.316215459504541</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78">
         <v>70.792542507934584</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="1">
+      <c r="A79">
         <v>78</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79">
         <v>23.023275417495121</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79">
         <v>72.572161398286397</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="1">
+      <c r="A80">
         <v>79</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80">
         <v>22.981828709336209</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80">
         <v>72.603659710311931</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="1">
+      <c r="A81">
         <v>80</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81">
         <v>22.458842062625109</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81">
         <v>70.056888162040678</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="1">
+      <c r="A82">
         <v>81</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82">
         <v>21.230412907706491</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82">
         <v>72.889632421951333</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="1">
+      <c r="A83">
         <v>82</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83">
         <v>21.21808107181365</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C83">
         <v>72.881469625656166</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="1">
+      <c r="A84">
         <v>83</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84">
         <v>22.298215318140318</v>
       </c>
-      <c r="C84" s="1">
+      <c r="C84">
         <v>70.795467813491825</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="1">
+      <c r="A85">
         <v>84</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85">
         <v>21.246777856847078</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C85">
         <v>72.891009970569613</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="1">
+      <c r="A86">
         <v>85</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86">
         <v>21.196140686344279</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86">
         <v>72.780127523803756</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="1">
+      <c r="A87">
         <v>86</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87">
         <v>23.02935139423521</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87">
         <v>72.467025656414052</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="1">
+      <c r="A88">
         <v>87</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88">
         <v>21.21746072645459</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C88">
         <v>72.894130753303557</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="1">
+      <c r="A89">
         <v>88</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89">
         <v>21.22298529335621</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C89">
         <v>72.788432462635029</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="1">
+      <c r="A90">
         <v>89</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90">
         <v>21.76543479754643</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C90">
         <v>70.621954753303555</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="1">
+      <c r="A91">
         <v>90</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91">
         <v>23.068786345046771</v>
       </c>
-      <c r="C91" s="1">
+      <c r="C91">
         <v>72.53798163194655</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="1">
+      <c r="A92">
         <v>91</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92">
         <v>21.216424410148331</v>
       </c>
-      <c r="C92" s="1">
+      <c r="C92">
         <v>72.893926614749901</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="1">
+      <c r="A93">
         <v>92</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93">
         <v>21.22179657295737</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C93">
         <v>72.883322159385727</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="1">
+      <c r="A94">
         <v>93</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94">
         <v>22.2890372446181</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94">
         <v>70.793497261238144</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="1">
+      <c r="A95">
         <v>94</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95">
         <v>21.22392771090696</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C95">
         <v>72.819630212303153</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="1">
+      <c r="A96">
         <v>95</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96">
         <v>21.224728158467311</v>
       </c>
-      <c r="C96" s="1">
+      <c r="C96">
         <v>72.819182283397694</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="1">
+      <c r="A97">
         <v>96</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97">
         <v>22.84952067161149</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97">
         <v>72.389614576721172</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="1">
+      <c r="A98">
         <v>97</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98">
         <v>21.233763124136178</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98">
         <v>72.904307231807735</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="1">
+      <c r="A99">
         <v>98</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99">
         <v>21.208100540362562</v>
       </c>
-      <c r="C99" s="1">
+      <c r="C99">
         <v>72.875286996364579</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" s="1">
+      <c r="A100">
         <v>99</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100">
         <v>21.131216610014551</v>
       </c>
-      <c r="C100" s="1">
+      <c r="C100">
         <v>72.890186238098124</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="1">
+      <c r="A101">
         <v>100</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101">
         <v>22.314386975239461</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101">
         <v>70.81857696924213</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="1">
+      <c r="A102">
         <v>101</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102">
         <v>23.011648114904471</v>
       </c>
-      <c r="C102" s="1">
+      <c r="C102">
         <v>72.641233295631437</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="1">
+      <c r="A103">
         <v>102</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103">
         <v>22.29489025897286</v>
       </c>
-      <c r="C103" s="1">
+      <c r="C103">
         <v>70.756987403774232</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="1">
+      <c r="A104">
         <v>103</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104">
         <v>23.062681990182998</v>
       </c>
-      <c r="C104" s="1">
+      <c r="C104">
         <v>72.52304134225848</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="1">
+      <c r="A105">
         <v>104</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105">
         <v>23.074306857733681</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105">
         <v>72.548291896820118</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" s="1">
+      <c r="A106">
         <v>105</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106">
         <v>21.14703347789559</v>
       </c>
-      <c r="C106" s="1">
+      <c r="C106">
         <v>72.869254402446742</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="1">
+      <c r="A107">
         <v>106</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107">
         <v>23.048694378319489</v>
       </c>
-      <c r="C107" s="1">
+      <c r="C107">
         <v>72.531880115413642</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="1">
+      <c r="A108">
         <v>107</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108">
         <v>21.216919550350319</v>
       </c>
-      <c r="C108" s="1">
+      <c r="C108">
         <v>72.892932111778222</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="1">
+      <c r="A109">
         <v>108</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109">
         <v>22.987981127324741</v>
       </c>
-      <c r="C109" s="1">
+      <c r="C109">
         <v>72.621955160713213</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="1">
+      <c r="A110">
         <v>109</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110">
         <v>21.224334779314791</v>
       </c>
-      <c r="C110" s="1">
+      <c r="C110">
         <v>72.826593119049065</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" s="1">
+      <c r="A111">
         <v>110</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B111">
         <v>22.280610100314341</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111">
         <v>70.761245654106091</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="1">
+      <c r="A112">
         <v>111</v>
       </c>
-      <c r="B112" s="1">
+      <c r="B112">
         <v>21.215917174938269</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112">
         <v>72.89188758895493</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="1">
+      <c r="A113">
         <v>112</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113">
         <v>23.047609515245281</v>
       </c>
-      <c r="C113" s="1">
+      <c r="C113">
         <v>72.645900549598721</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="1">
+      <c r="A114">
         <v>113</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114">
         <v>23.027704375199871</v>
       </c>
-      <c r="C114" s="1">
+      <c r="C114">
         <v>72.651243617057844</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="1">
+      <c r="A115">
         <v>114</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115">
         <v>21.135945157254831</v>
       </c>
-      <c r="C115" s="1">
+      <c r="C115">
         <v>72.799645541000388</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="1">
+      <c r="A116">
         <v>115</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116">
         <v>22.45742228020487</v>
       </c>
-      <c r="C116" s="1">
+      <c r="C116">
         <v>70.06594367361069</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="1">
+      <c r="A117">
         <v>116</v>
       </c>
-      <c r="B117" s="1">
+      <c r="B117">
         <v>21.23644094795635</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117">
         <v>72.909931077384925</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A118" s="1">
+      <c r="A118">
         <v>117</v>
       </c>
-      <c r="B118" s="1">
+      <c r="B118">
         <v>21.2402228338306</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118">
         <v>72.908097725200633</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A119" s="1">
+      <c r="A119">
         <v>118</v>
       </c>
-      <c r="B119" s="1">
+      <c r="B119">
         <v>21.237167092236941</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119">
         <v>72.886001867389709</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A120" s="1">
+      <c r="A120">
         <v>119</v>
       </c>
-      <c r="B120" s="1">
+      <c r="B120">
         <v>23.074244121390841</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120">
         <v>72.647372012233745</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="1">
+      <c r="A121">
         <v>120</v>
       </c>
-      <c r="B121" s="1">
+      <c r="B121">
         <v>22.269284873559521</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121">
         <v>70.768468164348633</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A122" s="1">
+      <c r="A122">
         <v>121</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122">
         <v>23.055606222713209</v>
       </c>
-      <c r="C122" s="1">
+      <c r="C122">
         <v>72.671632537364971</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A123" s="1">
+      <c r="A123">
         <v>122</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123">
         <v>23.119025166985018</v>
       </c>
-      <c r="C123" s="1">
+      <c r="C123">
         <v>72.57685475330355</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A124" s="1">
+      <c r="A124">
         <v>123</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124">
         <v>21.157127061233801</v>
       </c>
-      <c r="C124" s="1">
+      <c r="C124">
         <v>72.777243076057431</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A125" s="1">
+      <c r="A125">
         <v>124</v>
       </c>
-      <c r="B125" s="1">
+      <c r="B125">
         <v>21.211410880761431</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125">
         <v>72.783182770500204</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" s="1">
+      <c r="A126">
         <v>125</v>
       </c>
-      <c r="B126" s="1">
+      <c r="B126">
         <v>21.224322900425751</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126">
         <v>72.818755812164341</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" s="1">
+      <c r="A127">
         <v>126</v>
       </c>
-      <c r="B127" s="1">
+      <c r="B127">
         <v>21.218697792891081</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127">
         <v>72.881858545963297</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A128" s="1">
+      <c r="A128">
         <v>127</v>
       </c>
-      <c r="B128" s="1">
+      <c r="B128">
         <v>23.04040315698278</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128">
         <v>72.665788863754287</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A129" s="1">
+      <c r="A129">
         <v>128</v>
       </c>
-      <c r="B129" s="1">
+      <c r="B129">
         <v>21.229041425914541</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129">
         <v>72.824460875988038</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" s="1">
+      <c r="A130">
         <v>129</v>
       </c>
-      <c r="B130" s="1">
+      <c r="B130">
         <v>21.211846381610918</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130">
         <v>72.78355023313523</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A131" s="1">
+      <c r="A131">
         <v>130</v>
       </c>
-      <c r="B131" s="1">
+      <c r="B131">
         <v>23.073542232705801</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131">
         <v>72.650997261238146</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A132" s="1">
+      <c r="A132">
         <v>131</v>
       </c>
-      <c r="B132" s="1">
+      <c r="B132">
         <v>21.21941465266211</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132">
         <v>72.879582333660153</v>
       </c>
     </row>

</xml_diff>